<commit_message>
added zipcode-level NEVI, county --> borough, NVI --> NEVI
</commit_message>
<xml_diff>
--- a/tabs/prep-code-stab5.xlsx
+++ b/tabs/prep-code-stab5.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cumccolumbia-my.sharepoint.com/personal/spu2105_cumc_columbia_edu/Documents/Phi/My Courses/Columbia/Work/Research - Jeanette/projects/covid-vulnerability-index/comms/git nvi/tabs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F4F37F65-17C1-4E0D-8B30-F5C3F4361940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="8_{F4F37F65-17C1-4E0D-8B30-F5C3F4361940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9528EF0B-8723-416D-847D-572B5A0A5522}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{95DBCD7C-EEEB-4712-9BBA-7641E98E5657}"/>
+    <workbookView minimized="1" xWindow="12" yWindow="12" windowWidth="23016" windowHeight="12216" activeTab="1" xr2:uid="{95DBCD7C-EEEB-4712-9BBA-7641E98E5657}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="tab_fig" sheetId="1" r:id="rId1"/>
+    <sheet name="fig" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="78">
   <si>
     <t>score_demo_age</t>
   </si>
@@ -110,6 +111,162 @@
   </si>
   <si>
     <t>nvi</t>
+  </si>
+  <si>
+    <t>subdomain label</t>
+  </si>
+  <si>
+    <t>score_healthstatus_lackinsurance_median_iqr</t>
+  </si>
+  <si>
+    <t>score_healthstatus_preventive_median_iqr</t>
+  </si>
+  <si>
+    <t>score_healthstatus_condition_median_iqr</t>
+  </si>
+  <si>
+    <t>score_healthstatus_lifestyle_median_iqr</t>
+  </si>
+  <si>
+    <t>score_residential_vacancy_median_iqr</t>
+  </si>
+  <si>
+    <t>score_residential_move1yr_median_iqr</t>
+  </si>
+  <si>
+    <t>score_residential_structattach_median_iqr</t>
+  </si>
+  <si>
+    <t>score_residential_structage_median_iqr</t>
+  </si>
+  <si>
+    <t>score_residential_occperroom_median_iqr</t>
+  </si>
+  <si>
+    <t>score_residential_groupquarters_median_iqr</t>
+  </si>
+  <si>
+    <t>score_residential_popdensity_median_iqr</t>
+  </si>
+  <si>
+    <t>score_economic_vehicleavail_median_iqr</t>
+  </si>
+  <si>
+    <t>score_economic_education_median_iqr</t>
+  </si>
+  <si>
+    <t>score_economic_employment_median_iqr</t>
+  </si>
+  <si>
+    <t>score_economic_gini_median_iqr</t>
+  </si>
+  <si>
+    <t>score_economic_servicemanual_median_iqr</t>
+  </si>
+  <si>
+    <t>score_economic_incomepoverty_median_iqr</t>
+  </si>
+  <si>
+    <t>score_demo_livealone_median_iqr</t>
+  </si>
+  <si>
+    <t>score_demo_mobility_median_iqr</t>
+  </si>
+  <si>
+    <t>score_demo_singleparent_median_iqr</t>
+  </si>
+  <si>
+    <t>score_demo_disability_median_iqr</t>
+  </si>
+  <si>
+    <t>score_demo_immigration_median_iqr</t>
+  </si>
+  <si>
+    <t>score_demo_femaleled_median_iqr</t>
+  </si>
+  <si>
+    <t>score_demo_age_median_iqr</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Immigration</t>
+  </si>
+  <si>
+    <t>Disability</t>
+  </si>
+  <si>
+    <t>Mobility</t>
+  </si>
+  <si>
+    <t>Occupation</t>
+  </si>
+  <si>
+    <t>Unemployment</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>Vacancy</t>
+  </si>
+  <si>
+    <t>subdomain label code</t>
+  </si>
+  <si>
+    <t>OLD</t>
+  </si>
+  <si>
+    <t>Female-Led Households</t>
+  </si>
+  <si>
+    <t>Single Parent Households</t>
+  </si>
+  <si>
+    <t>Social Isolation</t>
+  </si>
+  <si>
+    <t>Income and Poverty</t>
+  </si>
+  <si>
+    <t>Income Inequality</t>
+  </si>
+  <si>
+    <t>Vehicle Availability</t>
+  </si>
+  <si>
+    <t>Population Density</t>
+  </si>
+  <si>
+    <t>Group Quarters</t>
+  </si>
+  <si>
+    <t>Occupants Per Room</t>
+  </si>
+  <si>
+    <t>Age of Housing Structure</t>
+  </si>
+  <si>
+    <t>Units in Housing Structure</t>
+  </si>
+  <si>
+    <t>Changing Residence</t>
+  </si>
+  <si>
+    <t>Unhealthy Behaviors</t>
+  </si>
+  <si>
+    <t>Health Outcomes</t>
+  </si>
+  <si>
+    <t>Prevention Practices</t>
+  </si>
+  <si>
+    <t>Health Insurance Access</t>
+  </si>
+  <si>
+    <t>row_no</t>
   </si>
 </sst>
 </file>
@@ -473,8 +630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75106F80-3848-40C7-9B92-C5A819A877C6}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -716,4 +873,499 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90FF50E7-1D64-428B-89B8-CDAD88077411}">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="str">
+        <f>"'"&amp;B2&amp;"',"</f>
+        <v>'Age',</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="str">
+        <f>"subdomain == '"&amp;A2&amp;"' ~ subdomain_label_vector["&amp;D2&amp;"],"</f>
+        <v>subdomain == 'score_demo_age_median_iqr' ~ subdomain_label_vector[1],</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C25" si="0">"'"&amp;B3&amp;"',"</f>
+        <v>'Female-Led Households',</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F25" si="1">"subdomain == '"&amp;A3&amp;"' ~ subdomain_label_vector["&amp;D3&amp;"],"</f>
+        <v>subdomain == 'score_demo_femaleled_median_iqr' ~ subdomain_label_vector[2],</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>'Immigration',</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="1"/>
+        <v>subdomain == 'score_demo_immigration_median_iqr' ~ subdomain_label_vector[3],</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>'Disability',</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="1"/>
+        <v>subdomain == 'score_demo_disability_median_iqr' ~ subdomain_label_vector[4],</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>'Single Parent Households',</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="1"/>
+        <v>subdomain == 'score_demo_singleparent_median_iqr' ~ subdomain_label_vector[5],</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>'Mobility',</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="1"/>
+        <v>subdomain == 'score_demo_mobility_median_iqr' ~ subdomain_label_vector[6],</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>'Social Isolation',</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="1"/>
+        <v>subdomain == 'score_demo_livealone_median_iqr' ~ subdomain_label_vector[7],</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>'Income and Poverty',</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="1"/>
+        <v>subdomain == 'score_economic_incomepoverty_median_iqr' ~ subdomain_label_vector[8],</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>'Occupation',</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="1"/>
+        <v>subdomain == 'score_economic_servicemanual_median_iqr' ~ subdomain_label_vector[9],</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>'Income Inequality',</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="1"/>
+        <v>subdomain == 'score_economic_gini_median_iqr' ~ subdomain_label_vector[10],</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>'Unemployment',</v>
+      </c>
+      <c r="D12">
+        <v>11</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="1"/>
+        <v>subdomain == 'score_economic_employment_median_iqr' ~ subdomain_label_vector[11],</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>'Education',</v>
+      </c>
+      <c r="D13">
+        <v>12</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="1"/>
+        <v>subdomain == 'score_economic_education_median_iqr' ~ subdomain_label_vector[12],</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>'Vehicle Availability',</v>
+      </c>
+      <c r="D14">
+        <v>13</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="1"/>
+        <v>subdomain == 'score_economic_vehicleavail_median_iqr' ~ subdomain_label_vector[13],</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>'Population Density',</v>
+      </c>
+      <c r="D15">
+        <v>14</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="1"/>
+        <v>subdomain == 'score_residential_popdensity_median_iqr' ~ subdomain_label_vector[14],</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>'Group Quarters',</v>
+      </c>
+      <c r="D16">
+        <v>15</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="1"/>
+        <v>subdomain == 'score_residential_groupquarters_median_iqr' ~ subdomain_label_vector[15],</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>'Occupants Per Room',</v>
+      </c>
+      <c r="D17">
+        <v>16</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="1"/>
+        <v>subdomain == 'score_residential_occperroom_median_iqr' ~ subdomain_label_vector[16],</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>'Age of Housing Structure',</v>
+      </c>
+      <c r="D18">
+        <v>17</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="1"/>
+        <v>subdomain == 'score_residential_structage_median_iqr' ~ subdomain_label_vector[17],</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>'Units in Housing Structure',</v>
+      </c>
+      <c r="D19">
+        <v>18</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="1"/>
+        <v>subdomain == 'score_residential_structattach_median_iqr' ~ subdomain_label_vector[18],</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>'Changing Residence',</v>
+      </c>
+      <c r="D20">
+        <v>19</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="1"/>
+        <v>subdomain == 'score_residential_move1yr_median_iqr' ~ subdomain_label_vector[19],</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>'Vacancy',</v>
+      </c>
+      <c r="D21">
+        <v>20</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="1"/>
+        <v>subdomain == 'score_residential_vacancy_median_iqr' ~ subdomain_label_vector[20],</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>'Unhealthy Behaviors',</v>
+      </c>
+      <c r="D22">
+        <v>21</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="1"/>
+        <v>subdomain == 'score_healthstatus_lifestyle_median_iqr' ~ subdomain_label_vector[21],</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>'Health Outcomes',</v>
+      </c>
+      <c r="D23">
+        <v>22</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="1"/>
+        <v>subdomain == 'score_healthstatus_condition_median_iqr' ~ subdomain_label_vector[22],</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>'Prevention Practices',</v>
+      </c>
+      <c r="D24">
+        <v>23</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="1"/>
+        <v>subdomain == 'score_healthstatus_preventive_median_iqr' ~ subdomain_label_vector[23],</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>'Health Insurance Access',</v>
+      </c>
+      <c r="D25">
+        <v>24</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="1"/>
+        <v>subdomain == 'score_healthstatus_lackinsurance_median_iqr' ~ subdomain_label_vector[24],</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>